<commit_message>
Finished process with deduplication algo
</commit_message>
<xml_diff>
--- a/dmgreps/damaged_items_reports.xlsx
+++ b/dmgreps/damaged_items_reports.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4965" yWindow="690" windowWidth="23070" windowHeight="10815" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11835" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,17 +413,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="14.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="10.85546875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="12.85546875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="15.5703125" bestFit="1" customWidth="1" min="3" max="3"/>
     <col width="9.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="15" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="9.85546875" bestFit="1" customWidth="1" min="6" max="6"/>
@@ -479,7 +479,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>table</t>
+          <t>Door</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -489,37 +489,37 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>room308</t>
+          <t>Room 102</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>broken leg</t>
+          <t>Broken leg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BSCS31A</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Follow-up</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>table</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -529,117 +529,117 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>room308</t>
+          <t>Room 101</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>broken leg</t>
+          <t>Cracked surface</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BSCS31A</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>chair</t>
+          <t>Chair</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>room113</t>
+          <t>Room 101</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>broken leg</t>
+          <t>Broken leg</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>BSIT21A</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>aircon</t>
+          <t>Chair</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>20</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>cl3</t>
+          <t>Room 101</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>defective</t>
+          <t>Cracked surface</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>tech</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Follow-up</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>television</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -649,37 +649,37 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>room103</t>
+          <t>Room 103</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>blackout screen</t>
+          <t>Broken leg</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>bscs11a</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>television</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -689,37 +689,37 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>room103</t>
+          <t>Room 102</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>blackout screen</t>
+          <t>Loose hinge</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>bscs11a</t>
+          <t>Dana</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>electric fan</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -729,57 +729,57 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>room308</t>
+          <t>Room 102</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>broken socket</t>
+          <t>Broken leg</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BSCS31A</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-09-14</t>
+          <t>2025-09-15</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Follow-up</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>chair</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>114-39</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ROOM308</t>
+          <t>Room 101</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>broken leg</t>
+          <t>Cracked surface</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BSCS31A</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -789,17 +789,17 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Follow-up</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>floorboard</t>
+          <t>Table</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -807,14 +807,19 @@
           <t>N/A</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Room 101</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>cracked</t>
+          <t>Cracked surface</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>dominic</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -830,13 +835,33 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
           <t>2025-09-15</t>
@@ -844,45 +869,1645 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Fixed</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Door</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Room 101</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Room 101</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Door</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Room 101</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Door</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Chair</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Room 101</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Broken leg</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Cracked surface</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Follow-up</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Window</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Door</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Room 103</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Loose hinge</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Dana</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Table</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Room 102</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Scratched</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Charlie</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>chair</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>broken armchair</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>&amp; C:/Users/April/AppData/Local/Microsoft/WindowsApps/python3.13.exe "c:/Users/April/Documents/Academics/BSCS/3rd Year/1st Sem/IntSys/Activities/dmgreps/damageditemsreports.py"</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>kjhgf</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2025-09-15</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>204-25</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Room204</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>broken leg</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>bscs31a</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>

</xml_diff>